<commit_message>
Swaps message for body in send_order
</commit_message>
<xml_diff>
--- a/1_order.xlsx
+++ b/1_order.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4811</v>
+        <v>4869</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>4811</v>
+        <v>4869</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3475</v>
+        <v>3517</v>
       </c>
       <c r="C3" t="n">
         <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>41700</v>
+        <v>42204</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4277</v>
+        <v>4328</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>4277</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="5">

</xml_diff>